<commit_message>
Update public BEAVRS data files with correct tilt correction data
</commit_message>
<xml_diff>
--- a/measurements/detector_signals/cycle_1/161/radial_measurements_all.xlsx
+++ b/measurements/detector_signals/cycle_1/161/radial_measurements_all.xlsx
@@ -904,13 +904,13 @@
         <v>8</v>
       </c>
       <c r="F3" t="n">
-        <v>0.51998632237</v>
+        <v>0.508245648867</v>
       </c>
       <c r="G3" t="n">
         <v>0.508251936679</v>
       </c>
       <c r="H3" t="n">
-        <v>-0.0117343856908</v>
+        <v>6.2878123297e-06</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -930,13 +930,13 @@
         <v>10</v>
       </c>
       <c r="F4" t="n">
-        <v>0.622596162957</v>
+        <v>0.633570024496</v>
       </c>
       <c r="G4" t="n">
-        <v>0.635567531155</v>
+        <v>0.635567531156</v>
       </c>
       <c r="H4" t="n">
-        <v>0.0129713681985</v>
+        <v>0.00199750665966</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -956,13 +956,13 @@
         <v>7</v>
       </c>
       <c r="F5" t="n">
-        <v>0.690532719584</v>
+        <v>0.701599288685</v>
       </c>
       <c r="G5" t="n">
         <v>0.71034018188</v>
       </c>
       <c r="H5" t="n">
-        <v>0.0198074622957</v>
+        <v>0.008740893194859999</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -982,13 +982,13 @@
         <v>13</v>
       </c>
       <c r="F6" t="n">
-        <v>0.666216950391</v>
+        <v>0.678846256784</v>
       </c>
       <c r="G6" t="n">
         <v>0.691141798586</v>
       </c>
       <c r="H6" t="n">
-        <v>0.0249248481946</v>
+        <v>0.0122955418018</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1008,13 +1008,13 @@
         <v>15</v>
       </c>
       <c r="F7" t="n">
-        <v>0.690532719584</v>
+        <v>0.701599288685</v>
       </c>
       <c r="G7" t="n">
         <v>0.71034018188</v>
       </c>
       <c r="H7" t="n">
-        <v>0.0198074622957</v>
+        <v>0.008740893194859999</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1034,13 +1034,13 @@
         <v>9</v>
       </c>
       <c r="F8" t="n">
-        <v>0.622596162957</v>
+        <v>0.633570024496</v>
       </c>
       <c r="G8" t="n">
-        <v>0.635567531155</v>
+        <v>0.635567531156</v>
       </c>
       <c r="H8" t="n">
-        <v>0.0129713681985</v>
+        <v>0.00199750665966</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -1060,13 +1060,13 @@
         <v>18</v>
       </c>
       <c r="F9" t="n">
-        <v>0.51998632237</v>
+        <v>0.508245648867</v>
       </c>
       <c r="G9" t="n">
         <v>0.508251936679</v>
       </c>
       <c r="H9" t="n">
-        <v>-0.0117343856908</v>
+        <v>6.2878123297e-06</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1086,13 +1086,13 @@
         <v>11</v>
       </c>
       <c r="F10" t="n">
-        <v>0.536432909213</v>
+        <v>0.545710923476</v>
       </c>
       <c r="G10" t="n">
         <v>0.533512967329</v>
       </c>
       <c r="H10" t="n">
-        <v>-0.00291994188374</v>
+        <v>-0.0121979561466</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1112,13 +1112,13 @@
         <v>21</v>
       </c>
       <c r="F11" t="n">
-        <v>0.740153399232</v>
+        <v>0.7539584878659999</v>
       </c>
       <c r="G11" t="n">
         <v>0.757830919502</v>
       </c>
       <c r="H11" t="n">
-        <v>0.0176775202698</v>
+        <v>0.00387243163598</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -1138,13 +1138,13 @@
         <v>12</v>
       </c>
       <c r="F12" t="n">
-        <v>1.14402073566</v>
+        <v>1.16332001126</v>
       </c>
       <c r="G12" t="n">
         <v>1.14482990906</v>
       </c>
       <c r="H12" t="n">
-        <v>0.000809173400702</v>
+        <v>-0.018490102199</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -1164,13 +1164,13 @@
         <v>24</v>
       </c>
       <c r="F13" t="n">
-        <v>0.8081335310809999</v>
+        <v>0.822605739677</v>
       </c>
       <c r="G13" t="n">
         <v>0.834624452678</v>
       </c>
       <c r="H13" t="n">
-        <v>0.026490921597</v>
+        <v>0.0120187130012</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1190,13 +1190,13 @@
         <v>14</v>
       </c>
       <c r="F14" t="n">
-        <v>1.29924708381</v>
+        <v>1.21126960749</v>
       </c>
       <c r="G14" t="n">
         <v>1.18625799933</v>
       </c>
       <c r="H14" t="n">
-        <v>-0.112989084483</v>
+        <v>-0.0250116081629</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -1216,13 +1216,13 @@
         <v>27</v>
       </c>
       <c r="F15" t="n">
-        <v>0.8081335310809999</v>
+        <v>0.822605739677</v>
       </c>
       <c r="G15" t="n">
         <v>0.834624452678</v>
       </c>
       <c r="H15" t="n">
-        <v>0.026490921597</v>
+        <v>0.0120187130012</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1242,13 +1242,13 @@
         <v>29</v>
       </c>
       <c r="F16" t="n">
-        <v>1.14402073566</v>
+        <v>1.16332001126</v>
       </c>
       <c r="G16" t="n">
         <v>1.14482990906</v>
       </c>
       <c r="H16" t="n">
-        <v>0.000809173400702</v>
+        <v>-0.018490102199</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1268,13 +1268,13 @@
         <v>31</v>
       </c>
       <c r="F17" t="n">
-        <v>0.740153399232</v>
+        <v>0.7539584878659999</v>
       </c>
       <c r="G17" t="n">
         <v>0.757830919502</v>
       </c>
       <c r="H17" t="n">
-        <v>0.0176775202698</v>
+        <v>0.00387243163598</v>
       </c>
     </row>
     <row r="18" spans="1:10">
@@ -1294,13 +1294,13 @@
         <v>33</v>
       </c>
       <c r="F18" t="n">
-        <v>0.536432909213</v>
+        <v>0.545710923476</v>
       </c>
       <c r="G18" t="n">
         <v>0.533512967329</v>
       </c>
       <c r="H18" t="n">
-        <v>-0.00291994188374</v>
+        <v>-0.0121979561466</v>
       </c>
     </row>
     <row r="19" spans="1:10">
@@ -1320,13 +1320,13 @@
         <v>35</v>
       </c>
       <c r="F19" t="n">
-        <v>0.536432909213</v>
+        <v>0.545710923476</v>
       </c>
       <c r="G19" t="n">
         <v>0.533512967329</v>
       </c>
       <c r="H19" t="n">
-        <v>-0.00291994188374</v>
+        <v>-0.0121979561466</v>
       </c>
     </row>
     <row r="20" spans="1:10">
@@ -1346,13 +1346,13 @@
         <v>37</v>
       </c>
       <c r="F20" t="n">
-        <v>0.6747973981249999</v>
+        <v>0.687179174242</v>
       </c>
       <c r="G20" t="n">
         <v>0.675985180196</v>
       </c>
       <c r="H20" t="n">
-        <v>0.0011877820706</v>
+        <v>-0.0111939940462</v>
       </c>
     </row>
     <row r="21" spans="1:10">
@@ -1372,13 +1372,13 @@
         <v>39</v>
       </c>
       <c r="F21" t="n">
-        <v>0.967927045037</v>
+        <v>0.984686311592</v>
       </c>
       <c r="G21" t="n">
-        <v>0.986190636578</v>
+        <v>0.986190636579</v>
       </c>
       <c r="H21" t="n">
-        <v>0.0182635915413</v>
+        <v>0.00150432498658</v>
       </c>
     </row>
     <row r="22" spans="1:10">
@@ -1398,13 +1398,13 @@
         <v>41</v>
       </c>
       <c r="F22" t="n">
-        <v>1.2135475467</v>
+        <v>1.23228780065</v>
       </c>
       <c r="G22" t="n">
         <v>1.23071741327</v>
       </c>
       <c r="H22" t="n">
-        <v>0.0171698665709</v>
+        <v>-0.00157038737878</v>
       </c>
     </row>
     <row r="23" spans="1:10">
@@ -1424,13 +1424,13 @@
         <v>16</v>
       </c>
       <c r="F23" t="n">
-        <v>0.9847901815</v>
+        <v>1.00188841038</v>
       </c>
       <c r="G23" t="n">
-        <v>0.997305490064</v>
+        <v>0.997305490065</v>
       </c>
       <c r="H23" t="n">
-        <v>0.0125153085644</v>
+        <v>-0.00458292031539</v>
       </c>
     </row>
     <row r="24" spans="1:10">
@@ -1450,13 +1450,13 @@
         <v>44</v>
       </c>
       <c r="F24" t="n">
-        <v>1.2135475467</v>
+        <v>1.23228780065</v>
       </c>
       <c r="G24" t="n">
         <v>1.23071741327</v>
       </c>
       <c r="H24" t="n">
-        <v>0.0171698665709</v>
+        <v>-0.00157038737878</v>
       </c>
     </row>
     <row r="25" spans="1:10">
@@ -1476,13 +1476,13 @@
         <v>17</v>
       </c>
       <c r="F25" t="n">
-        <v>0.967927045037</v>
+        <v>0.984686311592</v>
       </c>
       <c r="G25" t="n">
-        <v>0.986190636578</v>
+        <v>0.986190636579</v>
       </c>
       <c r="H25" t="n">
-        <v>0.0182635915413</v>
+        <v>0.00150432498658</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -1502,13 +1502,13 @@
         <v>47</v>
       </c>
       <c r="F26" t="n">
-        <v>0.6747973981249999</v>
+        <v>0.687179174242</v>
       </c>
       <c r="G26" t="n">
         <v>0.675985180196</v>
       </c>
       <c r="H26" t="n">
-        <v>0.0011877820706</v>
+        <v>-0.0111939940462</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -1528,13 +1528,13 @@
         <v>19</v>
       </c>
       <c r="F27" t="n">
-        <v>0.536432909213</v>
+        <v>0.545710923476</v>
       </c>
       <c r="G27" t="n">
         <v>0.533512967329</v>
       </c>
       <c r="H27" t="n">
-        <v>-0.00291994188374</v>
+        <v>-0.0121979561466</v>
       </c>
     </row>
     <row r="28" spans="1:10">
@@ -1554,13 +1554,13 @@
         <v>20</v>
       </c>
       <c r="F28" t="n">
-        <v>0.740153399232</v>
+        <v>0.7539584878659999</v>
       </c>
       <c r="G28" t="n">
         <v>0.757830919502</v>
       </c>
       <c r="H28" t="n">
-        <v>0.0176775202698</v>
+        <v>0.00387243163598</v>
       </c>
     </row>
     <row r="29" spans="1:10">
@@ -1580,13 +1580,13 @@
         <v>51</v>
       </c>
       <c r="F29" t="n">
-        <v>1.3157090422</v>
+        <v>1.29136388046</v>
       </c>
       <c r="G29" t="n">
         <v>1.28427079825</v>
       </c>
       <c r="H29" t="n">
-        <v>-0.031438243951</v>
+        <v>-0.00709308221064</v>
       </c>
     </row>
     <row r="30" spans="1:10">
@@ -1606,13 +1606,13 @@
         <v>53</v>
       </c>
       <c r="F30" t="n">
-        <v>1.1119078401</v>
+        <v>1.09169830677</v>
       </c>
       <c r="G30" t="n">
         <v>1.0882452004</v>
       </c>
       <c r="H30" t="n">
-        <v>-0.0236626396954</v>
+        <v>-0.00345310636515</v>
       </c>
     </row>
     <row r="31" spans="1:10">
@@ -1632,13 +1632,13 @@
         <v>22</v>
       </c>
       <c r="F31" t="n">
-        <v>1.28976963075</v>
+        <v>1.31079628805</v>
       </c>
       <c r="G31" t="n">
         <v>1.29841697541</v>
       </c>
       <c r="H31" t="n">
-        <v>0.008647344663060001</v>
+        <v>-0.0123793126366</v>
       </c>
     </row>
     <row r="32" spans="1:10">
@@ -1658,13 +1658,13 @@
         <v>56</v>
       </c>
       <c r="F32" t="n">
-        <v>1.1119078401</v>
+        <v>1.09169830677</v>
       </c>
       <c r="G32" t="n">
         <v>1.0882452004</v>
       </c>
       <c r="H32" t="n">
-        <v>-0.0236626396954</v>
+        <v>-0.00345310636515</v>
       </c>
     </row>
     <row r="33" spans="1:10">
@@ -1684,13 +1684,13 @@
         <v>58</v>
       </c>
       <c r="F33" t="n">
-        <v>1.3157090422</v>
+        <v>1.29136388046</v>
       </c>
       <c r="G33" t="n">
         <v>1.28427079825</v>
       </c>
       <c r="H33" t="n">
-        <v>-0.031438243951</v>
+        <v>-0.00709308221064</v>
       </c>
     </row>
     <row r="34" spans="1:10">
@@ -1710,13 +1710,13 @@
         <v>60</v>
       </c>
       <c r="F34" t="n">
-        <v>0.740153399232</v>
+        <v>0.7539584878659999</v>
       </c>
       <c r="G34" t="n">
         <v>0.757830919502</v>
       </c>
       <c r="H34" t="n">
-        <v>0.0176775202698</v>
+        <v>0.00387243163598</v>
       </c>
     </row>
     <row r="35" spans="1:10">
@@ -1736,13 +1736,13 @@
         <v>62</v>
       </c>
       <c r="F35" t="n">
-        <v>0.51998632237</v>
+        <v>0.508245648867</v>
       </c>
       <c r="G35" t="n">
         <v>0.508251936679</v>
       </c>
       <c r="H35" t="n">
-        <v>-0.0117343856908</v>
+        <v>6.2878123297e-06</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -1762,13 +1762,13 @@
         <v>23</v>
       </c>
       <c r="F36" t="n">
-        <v>1.31037353417</v>
+        <v>1.33211027851</v>
       </c>
       <c r="G36" t="n">
         <v>1.32974065342</v>
       </c>
       <c r="H36" t="n">
-        <v>0.0193671192491</v>
+        <v>-0.00236962509052</v>
       </c>
     </row>
     <row r="37" spans="1:10">
@@ -1788,13 +1788,13 @@
         <v>65</v>
       </c>
       <c r="F37" t="n">
-        <v>1.0909343795</v>
+        <v>1.11029862242</v>
       </c>
       <c r="G37" t="n">
         <v>1.12563152577</v>
       </c>
       <c r="H37" t="n">
-        <v>0.0346971462667</v>
+        <v>0.0153329033469</v>
       </c>
     </row>
     <row r="38" spans="1:10">
@@ -1814,13 +1814,13 @@
         <v>67</v>
       </c>
       <c r="F38" t="n">
-        <v>1.32658064091</v>
+        <v>1.34781485183</v>
       </c>
       <c r="G38" t="n">
         <v>1.34893903671</v>
       </c>
       <c r="H38" t="n">
-        <v>0.0223583958032</v>
+        <v>0.00112418488353</v>
       </c>
     </row>
     <row r="39" spans="1:10">
@@ -1840,13 +1840,13 @@
         <v>69</v>
       </c>
       <c r="F39" t="n">
-        <v>1.15180109192</v>
+        <v>1.12542156452</v>
       </c>
       <c r="G39" t="n">
         <v>1.1306837319</v>
       </c>
       <c r="H39" t="n">
-        <v>-0.0211173600233</v>
+        <v>0.00526216737696</v>
       </c>
     </row>
     <row r="40" spans="1:10">
@@ -1866,13 +1866,13 @@
         <v>71</v>
       </c>
       <c r="F40" t="n">
-        <v>1.32658064091</v>
+        <v>1.34781485183</v>
       </c>
       <c r="G40" t="n">
         <v>1.34893903671</v>
       </c>
       <c r="H40" t="n">
-        <v>0.0223583958032</v>
+        <v>0.00112418488353</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -1892,13 +1892,13 @@
         <v>73</v>
       </c>
       <c r="F41" t="n">
-        <v>1.0909343795</v>
+        <v>1.11029862242</v>
       </c>
       <c r="G41" t="n">
         <v>1.12563152577</v>
       </c>
       <c r="H41" t="n">
-        <v>0.0346971462667</v>
+        <v>0.0153329033469</v>
       </c>
     </row>
     <row r="42" spans="1:10">
@@ -1918,13 +1918,13 @@
         <v>25</v>
       </c>
       <c r="F42" t="n">
-        <v>1.31037353417</v>
+        <v>1.33211027851</v>
       </c>
       <c r="G42" t="n">
         <v>1.32974065342</v>
       </c>
       <c r="H42" t="n">
-        <v>0.0193671192491</v>
+        <v>-0.00236962509052</v>
       </c>
     </row>
     <row r="43" spans="1:10">
@@ -1944,13 +1944,13 @@
         <v>76</v>
       </c>
       <c r="F43" t="n">
-        <v>0.51998632237</v>
+        <v>0.508245648867</v>
       </c>
       <c r="G43" t="n">
         <v>0.508251936679</v>
       </c>
       <c r="H43" t="n">
-        <v>-0.0117343856908</v>
+        <v>6.2878123297e-06</v>
       </c>
     </row>
     <row r="44" spans="1:10">
@@ -1970,13 +1970,13 @@
         <v>26</v>
       </c>
       <c r="F44" t="n">
-        <v>0.622596162957</v>
+        <v>0.633570024496</v>
       </c>
       <c r="G44" t="n">
-        <v>0.635567531155</v>
+        <v>0.635567531156</v>
       </c>
       <c r="H44" t="n">
-        <v>0.0129713681985</v>
+        <v>0.00199750665966</v>
       </c>
     </row>
     <row r="45" spans="1:10">
@@ -1996,13 +1996,13 @@
         <v>79</v>
       </c>
       <c r="F45" t="n">
-        <v>1.14402073566</v>
+        <v>1.16332001126</v>
       </c>
       <c r="G45" t="n">
         <v>1.14482990906</v>
       </c>
       <c r="H45" t="n">
-        <v>0.000809173400702</v>
+        <v>-0.018490102199</v>
       </c>
     </row>
     <row r="46" spans="1:10">
@@ -2010,13 +2010,13 @@
         <v>28</v>
       </c>
       <c r="F46" t="n">
-        <v>0.967927045037</v>
+        <v>0.984686311592</v>
       </c>
       <c r="G46" t="n">
-        <v>0.986190636578</v>
+        <v>0.986190636579</v>
       </c>
       <c r="H46" t="n">
-        <v>0.0182635915413</v>
+        <v>0.00150432498658</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -2024,13 +2024,13 @@
         <v>80</v>
       </c>
       <c r="F47" t="n">
-        <v>1.3157090422</v>
+        <v>1.29136388046</v>
       </c>
       <c r="G47" t="n">
         <v>1.28427079825</v>
       </c>
       <c r="H47" t="n">
-        <v>-0.031438243951</v>
+        <v>-0.00709308221064</v>
       </c>
     </row>
     <row r="48" spans="1:10">
@@ -2038,13 +2038,13 @@
         <v>81</v>
       </c>
       <c r="F48" t="n">
-        <v>1.0909343795</v>
+        <v>1.11029862242</v>
       </c>
       <c r="G48" t="n">
         <v>1.12563152577</v>
       </c>
       <c r="H48" t="n">
-        <v>0.0346971462667</v>
+        <v>0.0153329033469</v>
       </c>
     </row>
     <row r="49" spans="1:10">
@@ -2052,13 +2052,13 @@
         <v>30</v>
       </c>
       <c r="F49" t="n">
-        <v>1.3561940674</v>
+        <v>1.3798652656</v>
       </c>
       <c r="G49" t="n">
         <v>1.36106433143</v>
       </c>
       <c r="H49" t="n">
-        <v>0.00487026402521</v>
+        <v>-0.0188009341744</v>
       </c>
     </row>
     <row r="50" spans="1:10">
@@ -2066,13 +2066,13 @@
         <v>82</v>
       </c>
       <c r="F50" t="n">
-        <v>1.13822314908</v>
+        <v>1.11355377866</v>
       </c>
       <c r="G50" t="n">
         <v>1.13169417312</v>
       </c>
       <c r="H50" t="n">
-        <v>-0.00652897595733</v>
+        <v>0.018140394463</v>
       </c>
     </row>
     <row r="51" spans="1:10">
@@ -2080,13 +2080,13 @@
         <v>32</v>
       </c>
       <c r="F51" t="n">
-        <v>1.36870167843</v>
+        <v>1.33892010145</v>
       </c>
       <c r="G51" t="n">
         <v>1.336813742</v>
       </c>
       <c r="H51" t="n">
-        <v>-0.0318879364288</v>
+        <v>-0.0021063594485</v>
       </c>
     </row>
     <row r="52" spans="1:10">
@@ -2094,13 +2094,13 @@
         <v>83</v>
       </c>
       <c r="F52" t="n">
-        <v>1.13822314908</v>
+        <v>1.11355377866</v>
       </c>
       <c r="G52" t="n">
         <v>1.13169417312</v>
       </c>
       <c r="H52" t="n">
-        <v>-0.00652897595733</v>
+        <v>0.018140394463</v>
       </c>
     </row>
     <row r="53" spans="1:10">
@@ -2108,13 +2108,13 @@
         <v>84</v>
       </c>
       <c r="F53" t="n">
-        <v>1.3561940674</v>
+        <v>1.3798652656</v>
       </c>
       <c r="G53" t="n">
         <v>1.36106433143</v>
       </c>
       <c r="H53" t="n">
-        <v>0.00487026402521</v>
+        <v>-0.0188009341744</v>
       </c>
     </row>
     <row r="54" spans="1:10">
@@ -2122,13 +2122,13 @@
         <v>85</v>
       </c>
       <c r="F54" t="n">
-        <v>1.0909343795</v>
+        <v>1.11029862242</v>
       </c>
       <c r="G54" t="n">
         <v>1.12563152577</v>
       </c>
       <c r="H54" t="n">
-        <v>0.0346971462667</v>
+        <v>0.0153329033469</v>
       </c>
     </row>
     <row r="55" spans="1:10">
@@ -2136,13 +2136,13 @@
         <v>86</v>
       </c>
       <c r="F55" t="n">
-        <v>1.3157090422</v>
+        <v>1.29136388046</v>
       </c>
       <c r="G55" t="n">
         <v>1.28427079825</v>
       </c>
       <c r="H55" t="n">
-        <v>-0.031438243951</v>
+        <v>-0.00709308221064</v>
       </c>
     </row>
     <row r="56" spans="1:10">
@@ -2150,13 +2150,13 @@
         <v>87</v>
       </c>
       <c r="F56" t="n">
-        <v>0.967927045037</v>
+        <v>0.984686311592</v>
       </c>
       <c r="G56" t="n">
-        <v>0.986190636578</v>
+        <v>0.986190636579</v>
       </c>
       <c r="H56" t="n">
-        <v>0.0182635915413</v>
+        <v>0.00150432498658</v>
       </c>
     </row>
     <row r="57" spans="1:10">
@@ -2164,13 +2164,13 @@
         <v>88</v>
       </c>
       <c r="F57" t="n">
-        <v>1.14402073566</v>
+        <v>1.16332001126</v>
       </c>
       <c r="G57" t="n">
         <v>1.14482990906</v>
       </c>
       <c r="H57" t="n">
-        <v>0.000809173400702</v>
+        <v>-0.018490102199</v>
       </c>
     </row>
     <row r="58" spans="1:10">
@@ -2178,13 +2178,13 @@
         <v>89</v>
       </c>
       <c r="F58" t="n">
-        <v>0.622596162957</v>
+        <v>0.633570024496</v>
       </c>
       <c r="G58" t="n">
-        <v>0.635567531155</v>
+        <v>0.635567531156</v>
       </c>
       <c r="H58" t="n">
-        <v>0.0129713681985</v>
+        <v>0.00199750665966</v>
       </c>
     </row>
     <row r="59" spans="1:10">
@@ -2192,13 +2192,13 @@
         <v>90</v>
       </c>
       <c r="F59" t="n">
-        <v>0.690532719584</v>
+        <v>0.701599288685</v>
       </c>
       <c r="G59" t="n">
         <v>0.71034018188</v>
       </c>
       <c r="H59" t="n">
-        <v>0.0198074622957</v>
+        <v>0.008740893194859999</v>
       </c>
     </row>
     <row r="60" spans="1:10">
@@ -2206,13 +2206,13 @@
         <v>91</v>
       </c>
       <c r="F60" t="n">
-        <v>0.8081335310809999</v>
+        <v>0.822605739677</v>
       </c>
       <c r="G60" t="n">
         <v>0.834624452678</v>
       </c>
       <c r="H60" t="n">
-        <v>0.026490921597</v>
+        <v>0.0120187130012</v>
       </c>
     </row>
     <row r="61" spans="1:10">
@@ -2220,13 +2220,13 @@
         <v>92</v>
       </c>
       <c r="F61" t="n">
-        <v>1.2135475467</v>
+        <v>1.23228780065</v>
       </c>
       <c r="G61" t="n">
         <v>1.23071741327</v>
       </c>
       <c r="H61" t="n">
-        <v>0.0171698665709</v>
+        <v>-0.00157038737878</v>
       </c>
     </row>
     <row r="62" spans="1:10">
@@ -2234,13 +2234,13 @@
         <v>34</v>
       </c>
       <c r="F62" t="n">
-        <v>1.1119078401</v>
+        <v>1.09169830677</v>
       </c>
       <c r="G62" t="n">
         <v>1.0882452004</v>
       </c>
       <c r="H62" t="n">
-        <v>-0.0236626396954</v>
+        <v>-0.00345310636515</v>
       </c>
     </row>
     <row r="63" spans="1:10">
@@ -2248,13 +2248,13 @@
         <v>93</v>
       </c>
       <c r="F63" t="n">
-        <v>1.32658064091</v>
+        <v>1.34781485183</v>
       </c>
       <c r="G63" t="n">
         <v>1.34893903671</v>
       </c>
       <c r="H63" t="n">
-        <v>0.0223583958032</v>
+        <v>0.00112418488353</v>
       </c>
     </row>
     <row r="64" spans="1:10">
@@ -2262,13 +2262,13 @@
         <v>94</v>
       </c>
       <c r="F64" t="n">
-        <v>1.13822314908</v>
+        <v>1.11355377866</v>
       </c>
       <c r="G64" t="n">
         <v>1.13169417312</v>
       </c>
       <c r="H64" t="n">
-        <v>-0.00652897595733</v>
+        <v>0.018140394463</v>
       </c>
     </row>
     <row r="65" spans="1:10">
@@ -2276,13 +2276,13 @@
         <v>95</v>
       </c>
       <c r="F65" t="n">
-        <v>1.43125236943</v>
+        <v>1.30139878445</v>
       </c>
       <c r="G65" t="n">
         <v>1.3095318289</v>
       </c>
       <c r="H65" t="n">
-        <v>-0.121720540531</v>
+        <v>0.008133044449429999</v>
       </c>
     </row>
     <row r="66" spans="1:10">
@@ -2290,13 +2290,13 @@
         <v>96</v>
       </c>
       <c r="F66" t="n">
-        <v>1.01348516684</v>
+        <v>1.03087691513</v>
       </c>
       <c r="G66" t="n">
         <v>1.04176490401</v>
       </c>
       <c r="H66" t="n">
-        <v>0.0282797371685</v>
+        <v>0.0108879888787</v>
       </c>
     </row>
     <row r="67" spans="1:10">
@@ -2304,13 +2304,13 @@
         <v>97</v>
       </c>
       <c r="F67" t="n">
-        <v>1.43125236943</v>
+        <v>1.30139878445</v>
       </c>
       <c r="G67" t="n">
         <v>1.3095318289</v>
       </c>
       <c r="H67" t="n">
-        <v>-0.121720540531</v>
+        <v>0.008133044449429999</v>
       </c>
     </row>
     <row r="68" spans="1:10">
@@ -2318,13 +2318,13 @@
         <v>36</v>
       </c>
       <c r="F68" t="n">
-        <v>1.13822314908</v>
+        <v>1.11355377866</v>
       </c>
       <c r="G68" t="n">
         <v>1.13169417312</v>
       </c>
       <c r="H68" t="n">
-        <v>-0.00652897595733</v>
+        <v>0.018140394463</v>
       </c>
     </row>
     <row r="69" spans="1:10">
@@ -2332,13 +2332,13 @@
         <v>98</v>
       </c>
       <c r="F69" t="n">
-        <v>1.32658064091</v>
+        <v>1.34781485183</v>
       </c>
       <c r="G69" t="n">
         <v>1.34893903671</v>
       </c>
       <c r="H69" t="n">
-        <v>0.0223583958032</v>
+        <v>0.00112418488353</v>
       </c>
     </row>
     <row r="70" spans="1:10">
@@ -2346,13 +2346,13 @@
         <v>99</v>
       </c>
       <c r="F70" t="n">
-        <v>1.1119078401</v>
+        <v>1.09169830677</v>
       </c>
       <c r="G70" t="n">
         <v>1.0882452004</v>
       </c>
       <c r="H70" t="n">
-        <v>-0.0236626396954</v>
+        <v>-0.00345310636515</v>
       </c>
     </row>
     <row r="71" spans="1:10">
@@ -2360,13 +2360,13 @@
         <v>38</v>
       </c>
       <c r="F71" t="n">
-        <v>1.2135475467</v>
+        <v>1.23228780065</v>
       </c>
       <c r="G71" t="n">
         <v>1.23071741327</v>
       </c>
       <c r="H71" t="n">
-        <v>0.0171698665709</v>
+        <v>-0.00157038737878</v>
       </c>
     </row>
     <row r="72" spans="1:10">
@@ -2374,13 +2374,13 @@
         <v>100</v>
       </c>
       <c r="F72" t="n">
-        <v>0.8081335310809999</v>
+        <v>0.822605739677</v>
       </c>
       <c r="G72" t="n">
         <v>0.834624452678</v>
       </c>
       <c r="H72" t="n">
-        <v>0.026490921597</v>
+        <v>0.0120187130012</v>
       </c>
     </row>
     <row r="73" spans="1:10">
@@ -2388,13 +2388,13 @@
         <v>101</v>
       </c>
       <c r="F73" t="n">
-        <v>0.690532719584</v>
+        <v>0.701599288685</v>
       </c>
       <c r="G73" t="n">
         <v>0.71034018188</v>
       </c>
       <c r="H73" t="n">
-        <v>0.0198074622957</v>
+        <v>0.008740893194859999</v>
       </c>
     </row>
     <row r="74" spans="1:10">
@@ -2402,13 +2402,13 @@
         <v>40</v>
       </c>
       <c r="F74" t="n">
-        <v>0.666216950391</v>
+        <v>0.678846256784</v>
       </c>
       <c r="G74" t="n">
         <v>0.691141798586</v>
       </c>
       <c r="H74" t="n">
-        <v>0.0249248481946</v>
+        <v>0.0122955418018</v>
       </c>
     </row>
     <row r="75" spans="1:10">
@@ -2416,13 +2416,13 @@
         <v>102</v>
       </c>
       <c r="F75" t="n">
-        <v>1.29924708381</v>
+        <v>1.21126960749</v>
       </c>
       <c r="G75" t="n">
         <v>1.18625799933</v>
       </c>
       <c r="H75" t="n">
-        <v>-0.112989084483</v>
+        <v>-0.0250116081629</v>
       </c>
     </row>
     <row r="76" spans="1:10">
@@ -2430,13 +2430,13 @@
         <v>42</v>
       </c>
       <c r="F76" t="n">
-        <v>0.9847901815</v>
+        <v>1.00188841038</v>
       </c>
       <c r="G76" t="n">
-        <v>0.997305490064</v>
+        <v>0.997305490065</v>
       </c>
       <c r="H76" t="n">
-        <v>0.0125153085644</v>
+        <v>-0.00458292031539</v>
       </c>
     </row>
     <row r="77" spans="1:10">
@@ -2444,13 +2444,13 @@
         <v>103</v>
       </c>
       <c r="F77" t="n">
-        <v>1.28976963075</v>
+        <v>1.31079628805</v>
       </c>
       <c r="G77" t="n">
         <v>1.29841697541</v>
       </c>
       <c r="H77" t="n">
-        <v>0.008647344663060001</v>
+        <v>-0.0123793126366</v>
       </c>
     </row>
     <row r="78" spans="1:10">
@@ -2458,13 +2458,13 @@
         <v>43</v>
       </c>
       <c r="F78" t="n">
-        <v>1.15180109192</v>
+        <v>1.12542156452</v>
       </c>
       <c r="G78" t="n">
         <v>1.1306837319</v>
       </c>
       <c r="H78" t="n">
-        <v>-0.0211173600233</v>
+        <v>0.00526216737696</v>
       </c>
     </row>
     <row r="79" spans="1:10">
@@ -2472,13 +2472,13 @@
         <v>104</v>
       </c>
       <c r="F79" t="n">
-        <v>1.36870167843</v>
+        <v>1.33892010145</v>
       </c>
       <c r="G79" t="n">
         <v>1.336813742</v>
       </c>
       <c r="H79" t="n">
-        <v>-0.0318879364288</v>
+        <v>-0.0021063594485</v>
       </c>
     </row>
     <row r="80" spans="1:10">
@@ -2486,13 +2486,13 @@
         <v>45</v>
       </c>
       <c r="F80" t="n">
-        <v>1.01348516684</v>
+        <v>1.03087691513</v>
       </c>
       <c r="G80" t="n">
         <v>1.04176490401</v>
       </c>
       <c r="H80" t="n">
-        <v>0.0282797371685</v>
+        <v>0.0108879888787</v>
       </c>
     </row>
     <row r="81" spans="1:10">
@@ -2500,13 +2500,13 @@
         <v>105</v>
       </c>
       <c r="F81" t="n">
-        <v>1.01348516684</v>
+        <v>1.03087691513</v>
       </c>
       <c r="G81" t="n">
         <v>1.04176490401</v>
       </c>
       <c r="H81" t="n">
-        <v>0.0282797371685</v>
+        <v>0.0108879888787</v>
       </c>
     </row>
     <row r="82" spans="1:10">
@@ -2514,13 +2514,13 @@
         <v>46</v>
       </c>
       <c r="F82" t="n">
-        <v>1.36870167843</v>
+        <v>1.33892010145</v>
       </c>
       <c r="G82" t="n">
         <v>1.336813742</v>
       </c>
       <c r="H82" t="n">
-        <v>-0.0318879364288</v>
+        <v>-0.0021063594485</v>
       </c>
     </row>
     <row r="83" spans="1:10">
@@ -2528,13 +2528,13 @@
         <v>106</v>
       </c>
       <c r="F83" t="n">
-        <v>1.15180109192</v>
+        <v>1.12542156452</v>
       </c>
       <c r="G83" t="n">
         <v>1.1306837319</v>
       </c>
       <c r="H83" t="n">
-        <v>-0.0211173600233</v>
+        <v>0.00526216737696</v>
       </c>
     </row>
     <row r="84" spans="1:10">
@@ -2542,13 +2542,13 @@
         <v>48</v>
       </c>
       <c r="F84" t="n">
-        <v>1.28976963075</v>
+        <v>1.31079628805</v>
       </c>
       <c r="G84" t="n">
         <v>1.29841697541</v>
       </c>
       <c r="H84" t="n">
-        <v>0.008647344663060001</v>
+        <v>-0.0123793126366</v>
       </c>
     </row>
     <row r="85" spans="1:10">
@@ -2556,13 +2556,13 @@
         <v>107</v>
       </c>
       <c r="F85" t="n">
-        <v>0.9847901815</v>
+        <v>1.00188841038</v>
       </c>
       <c r="G85" t="n">
-        <v>0.997305490064</v>
+        <v>0.997305490065</v>
       </c>
       <c r="H85" t="n">
-        <v>0.0125153085644</v>
+        <v>-0.00458292031539</v>
       </c>
     </row>
     <row r="86" spans="1:10">
@@ -2570,13 +2570,13 @@
         <v>108</v>
       </c>
       <c r="F86" t="n">
-        <v>1.29924708381</v>
+        <v>1.21126960749</v>
       </c>
       <c r="G86" t="n">
         <v>1.18625799933</v>
       </c>
       <c r="H86" t="n">
-        <v>-0.112989084483</v>
+        <v>-0.0250116081629</v>
       </c>
     </row>
     <row r="87" spans="1:10">
@@ -2584,13 +2584,13 @@
         <v>109</v>
       </c>
       <c r="F87" t="n">
-        <v>0.666216950391</v>
+        <v>0.678846256784</v>
       </c>
       <c r="G87" t="n">
         <v>0.691141798586</v>
       </c>
       <c r="H87" t="n">
-        <v>0.0249248481946</v>
+        <v>0.0122955418018</v>
       </c>
     </row>
     <row r="88" spans="1:10">
@@ -2598,13 +2598,13 @@
         <v>110</v>
       </c>
       <c r="F88" t="n">
-        <v>0.690532719584</v>
+        <v>0.701599288685</v>
       </c>
       <c r="G88" t="n">
         <v>0.71034018188</v>
       </c>
       <c r="H88" t="n">
-        <v>0.0198074622957</v>
+        <v>0.008740893194859999</v>
       </c>
     </row>
     <row r="89" spans="1:10">
@@ -2612,13 +2612,13 @@
         <v>49</v>
       </c>
       <c r="F89" t="n">
-        <v>0.8081335310809999</v>
+        <v>0.822605739677</v>
       </c>
       <c r="G89" t="n">
         <v>0.834624452678</v>
       </c>
       <c r="H89" t="n">
-        <v>0.026490921597</v>
+        <v>0.0120187130012</v>
       </c>
     </row>
     <row r="90" spans="1:10">
@@ -2626,13 +2626,13 @@
         <v>111</v>
       </c>
       <c r="F90" t="n">
-        <v>1.2135475467</v>
+        <v>1.23228780065</v>
       </c>
       <c r="G90" t="n">
         <v>1.23071741327</v>
       </c>
       <c r="H90" t="n">
-        <v>0.0171698665709</v>
+        <v>-0.00157038737878</v>
       </c>
     </row>
     <row r="91" spans="1:10">
@@ -2640,13 +2640,13 @@
         <v>112</v>
       </c>
       <c r="F91" t="n">
-        <v>1.1119078401</v>
+        <v>1.09169830677</v>
       </c>
       <c r="G91" t="n">
         <v>1.0882452004</v>
       </c>
       <c r="H91" t="n">
-        <v>-0.0236626396954</v>
+        <v>-0.00345310636515</v>
       </c>
     </row>
     <row r="92" spans="1:10">
@@ -2654,13 +2654,13 @@
         <v>113</v>
       </c>
       <c r="F92" t="n">
-        <v>1.32658064091</v>
+        <v>1.34781485183</v>
       </c>
       <c r="G92" t="n">
         <v>1.34893903671</v>
       </c>
       <c r="H92" t="n">
-        <v>0.0223583958032</v>
+        <v>0.00112418488353</v>
       </c>
     </row>
     <row r="93" spans="1:10">
@@ -2668,13 +2668,13 @@
         <v>114</v>
       </c>
       <c r="F93" t="n">
-        <v>1.13822314908</v>
+        <v>1.11355377866</v>
       </c>
       <c r="G93" t="n">
         <v>1.13169417312</v>
       </c>
       <c r="H93" t="n">
-        <v>-0.00652897595733</v>
+        <v>0.018140394463</v>
       </c>
     </row>
     <row r="94" spans="1:10">
@@ -2682,13 +2682,13 @@
         <v>115</v>
       </c>
       <c r="F94" t="n">
-        <v>1.43125236943</v>
+        <v>1.30139878445</v>
       </c>
       <c r="G94" t="n">
         <v>1.3095318289</v>
       </c>
       <c r="H94" t="n">
-        <v>-0.121720540531</v>
+        <v>0.008133044449429999</v>
       </c>
     </row>
     <row r="95" spans="1:10">
@@ -2696,13 +2696,13 @@
         <v>116</v>
       </c>
       <c r="F95" t="n">
-        <v>1.01348516684</v>
+        <v>1.03087691513</v>
       </c>
       <c r="G95" t="n">
         <v>1.04176490401</v>
       </c>
       <c r="H95" t="n">
-        <v>0.0282797371685</v>
+        <v>0.0108879888787</v>
       </c>
     </row>
     <row r="96" spans="1:10">
@@ -2710,13 +2710,13 @@
         <v>50</v>
       </c>
       <c r="F96" t="n">
-        <v>1.43125236943</v>
+        <v>1.30139878445</v>
       </c>
       <c r="G96" t="n">
         <v>1.3095318289</v>
       </c>
       <c r="H96" t="n">
-        <v>-0.121720540531</v>
+        <v>0.008133044449429999</v>
       </c>
     </row>
     <row r="97" spans="1:10">
@@ -2724,13 +2724,13 @@
         <v>117</v>
       </c>
       <c r="F97" t="n">
-        <v>1.13822314908</v>
+        <v>1.11355377866</v>
       </c>
       <c r="G97" t="n">
         <v>1.13169417312</v>
       </c>
       <c r="H97" t="n">
-        <v>-0.00652897595733</v>
+        <v>0.018140394463</v>
       </c>
     </row>
     <row r="98" spans="1:10">
@@ -2738,13 +2738,13 @@
         <v>52</v>
       </c>
       <c r="F98" t="n">
-        <v>1.32658064091</v>
+        <v>1.34781485183</v>
       </c>
       <c r="G98" t="n">
         <v>1.34893903671</v>
       </c>
       <c r="H98" t="n">
-        <v>0.0223583958032</v>
+        <v>0.00112418488353</v>
       </c>
     </row>
     <row r="99" spans="1:10">
@@ -2752,13 +2752,13 @@
         <v>118</v>
       </c>
       <c r="F99" t="n">
-        <v>1.1119078401</v>
+        <v>1.09169830677</v>
       </c>
       <c r="G99" t="n">
         <v>1.0882452004</v>
       </c>
       <c r="H99" t="n">
-        <v>-0.0236626396954</v>
+        <v>-0.00345310636515</v>
       </c>
     </row>
     <row r="100" spans="1:10">
@@ -2766,13 +2766,13 @@
         <v>119</v>
       </c>
       <c r="F100" t="n">
-        <v>1.2135475467</v>
+        <v>1.23228780065</v>
       </c>
       <c r="G100" t="n">
         <v>1.23071741327</v>
       </c>
       <c r="H100" t="n">
-        <v>0.0171698665709</v>
+        <v>-0.00157038737878</v>
       </c>
     </row>
     <row r="101" spans="1:10">
@@ -2780,13 +2780,13 @@
         <v>120</v>
       </c>
       <c r="F101" t="n">
-        <v>0.8081335310809999</v>
+        <v>0.822605739677</v>
       </c>
       <c r="G101" t="n">
         <v>0.834624452678</v>
       </c>
       <c r="H101" t="n">
-        <v>0.026490921597</v>
+        <v>0.0120187130012</v>
       </c>
     </row>
     <row r="102" spans="1:10">
@@ -2794,13 +2794,13 @@
         <v>54</v>
       </c>
       <c r="F102" t="n">
-        <v>0.690532719584</v>
+        <v>0.701599288685</v>
       </c>
       <c r="G102" t="n">
         <v>0.71034018188</v>
       </c>
       <c r="H102" t="n">
-        <v>0.0198074622957</v>
+        <v>0.008740893194859999</v>
       </c>
     </row>
     <row r="103" spans="1:10">
@@ -2808,13 +2808,13 @@
         <v>121</v>
       </c>
       <c r="F103" t="n">
-        <v>0.622596162957</v>
+        <v>0.633570024496</v>
       </c>
       <c r="G103" t="n">
-        <v>0.635567531155</v>
+        <v>0.635567531156</v>
       </c>
       <c r="H103" t="n">
-        <v>0.0129713681985</v>
+        <v>0.00199750665966</v>
       </c>
     </row>
     <row r="104" spans="1:10">
@@ -2822,13 +2822,13 @@
         <v>122</v>
       </c>
       <c r="F104" t="n">
-        <v>1.14402073566</v>
+        <v>1.16332001126</v>
       </c>
       <c r="G104" t="n">
         <v>1.14482990906</v>
       </c>
       <c r="H104" t="n">
-        <v>0.000809173400702</v>
+        <v>-0.018490102199</v>
       </c>
     </row>
     <row r="105" spans="1:10">
@@ -2836,13 +2836,13 @@
         <v>123</v>
       </c>
       <c r="F105" t="n">
-        <v>0.967927045037</v>
+        <v>0.984686311592</v>
       </c>
       <c r="G105" t="n">
-        <v>0.986190636578</v>
+        <v>0.986190636579</v>
       </c>
       <c r="H105" t="n">
-        <v>0.0182635915413</v>
+        <v>0.00150432498658</v>
       </c>
     </row>
     <row r="106" spans="1:10">
@@ -2850,13 +2850,13 @@
         <v>124</v>
       </c>
       <c r="F106" t="n">
-        <v>1.3157090422</v>
+        <v>1.29136388046</v>
       </c>
       <c r="G106" t="n">
         <v>1.28427079825</v>
       </c>
       <c r="H106" t="n">
-        <v>-0.031438243951</v>
+        <v>-0.00709308221064</v>
       </c>
     </row>
     <row r="107" spans="1:10">
@@ -2864,13 +2864,13 @@
         <v>55</v>
       </c>
       <c r="F107" t="n">
-        <v>1.0909343795</v>
+        <v>1.11029862242</v>
       </c>
       <c r="G107" t="n">
         <v>1.12563152577</v>
       </c>
       <c r="H107" t="n">
-        <v>0.0346971462667</v>
+        <v>0.0153329033469</v>
       </c>
     </row>
     <row r="108" spans="1:10">
@@ -2878,13 +2878,13 @@
         <v>125</v>
       </c>
       <c r="F108" t="n">
-        <v>1.3561940674</v>
+        <v>1.3798652656</v>
       </c>
       <c r="G108" t="n">
         <v>1.36106433143</v>
       </c>
       <c r="H108" t="n">
-        <v>0.00487026402521</v>
+        <v>-0.0188009341744</v>
       </c>
     </row>
     <row r="109" spans="1:10">
@@ -2892,13 +2892,13 @@
         <v>57</v>
       </c>
       <c r="F109" t="n">
-        <v>1.13822314908</v>
+        <v>1.11355377866</v>
       </c>
       <c r="G109" t="n">
         <v>1.13169417312</v>
       </c>
       <c r="H109" t="n">
-        <v>-0.00652897595733</v>
+        <v>0.018140394463</v>
       </c>
     </row>
     <row r="110" spans="1:10">
@@ -2906,13 +2906,13 @@
         <v>126</v>
       </c>
       <c r="F110" t="n">
-        <v>1.36870167843</v>
+        <v>1.33892010145</v>
       </c>
       <c r="G110" t="n">
         <v>1.336813742</v>
       </c>
       <c r="H110" t="n">
-        <v>-0.0318879364288</v>
+        <v>-0.0021063594485</v>
       </c>
     </row>
     <row r="111" spans="1:10">
@@ -2920,13 +2920,13 @@
         <v>127</v>
       </c>
       <c r="F111" t="n">
-        <v>1.13822314908</v>
+        <v>1.11355377866</v>
       </c>
       <c r="G111" t="n">
         <v>1.13169417312</v>
       </c>
       <c r="H111" t="n">
-        <v>-0.00652897595733</v>
+        <v>0.018140394463</v>
       </c>
     </row>
     <row r="112" spans="1:10">
@@ -2934,13 +2934,13 @@
         <v>128</v>
       </c>
       <c r="F112" t="n">
-        <v>1.3561940674</v>
+        <v>1.3798652656</v>
       </c>
       <c r="G112" t="n">
         <v>1.36106433143</v>
       </c>
       <c r="H112" t="n">
-        <v>0.00487026402521</v>
+        <v>-0.0188009341744</v>
       </c>
     </row>
     <row r="113" spans="1:10">
@@ -2948,13 +2948,13 @@
         <v>129</v>
       </c>
       <c r="F113" t="n">
-        <v>1.0909343795</v>
+        <v>1.11029862242</v>
       </c>
       <c r="G113" t="n">
         <v>1.12563152577</v>
       </c>
       <c r="H113" t="n">
-        <v>0.0346971462667</v>
+        <v>0.0153329033469</v>
       </c>
     </row>
     <row r="114" spans="1:10">
@@ -2962,13 +2962,13 @@
         <v>59</v>
       </c>
       <c r="F114" t="n">
-        <v>1.3157090422</v>
+        <v>1.29136388046</v>
       </c>
       <c r="G114" t="n">
         <v>1.28427079825</v>
       </c>
       <c r="H114" t="n">
-        <v>-0.031438243951</v>
+        <v>-0.00709308221064</v>
       </c>
     </row>
     <row r="115" spans="1:10">
@@ -2976,13 +2976,13 @@
         <v>130</v>
       </c>
       <c r="F115" t="n">
-        <v>0.967927045037</v>
+        <v>0.984686311592</v>
       </c>
       <c r="G115" t="n">
-        <v>0.986190636578</v>
+        <v>0.986190636579</v>
       </c>
       <c r="H115" t="n">
-        <v>0.0182635915413</v>
+        <v>0.00150432498658</v>
       </c>
     </row>
     <row r="116" spans="1:10">
@@ -2990,13 +2990,13 @@
         <v>131</v>
       </c>
       <c r="F116" t="n">
-        <v>1.14402073566</v>
+        <v>1.16332001126</v>
       </c>
       <c r="G116" t="n">
         <v>1.14482990906</v>
       </c>
       <c r="H116" t="n">
-        <v>0.000809173400702</v>
+        <v>-0.018490102199</v>
       </c>
     </row>
     <row r="117" spans="1:10">
@@ -3004,13 +3004,13 @@
         <v>132</v>
       </c>
       <c r="F117" t="n">
-        <v>0.622596162957</v>
+        <v>0.633570024496</v>
       </c>
       <c r="G117" t="n">
-        <v>0.635567531155</v>
+        <v>0.635567531156</v>
       </c>
       <c r="H117" t="n">
-        <v>0.0129713681985</v>
+        <v>0.00199750665966</v>
       </c>
     </row>
     <row r="118" spans="1:10">
@@ -3018,13 +3018,13 @@
         <v>133</v>
       </c>
       <c r="F118" t="n">
-        <v>0.51998632237</v>
+        <v>0.508245648867</v>
       </c>
       <c r="G118" t="n">
         <v>0.508251936679</v>
       </c>
       <c r="H118" t="n">
-        <v>-0.0117343856908</v>
+        <v>6.2878123297e-06</v>
       </c>
     </row>
     <row r="119" spans="1:10">
@@ -3032,13 +3032,13 @@
         <v>134</v>
       </c>
       <c r="F119" t="n">
-        <v>1.31037353417</v>
+        <v>1.33211027851</v>
       </c>
       <c r="G119" t="n">
         <v>1.32974065342</v>
       </c>
       <c r="H119" t="n">
-        <v>0.0193671192491</v>
+        <v>-0.00236962509052</v>
       </c>
     </row>
     <row r="120" spans="1:10">
@@ -3046,13 +3046,13 @@
         <v>135</v>
       </c>
       <c r="F120" t="n">
-        <v>1.0909343795</v>
+        <v>1.11029862242</v>
       </c>
       <c r="G120" t="n">
         <v>1.12563152577</v>
       </c>
       <c r="H120" t="n">
-        <v>0.0346971462667</v>
+        <v>0.0153329033469</v>
       </c>
     </row>
     <row r="121" spans="1:10">
@@ -3060,13 +3060,13 @@
         <v>136</v>
       </c>
       <c r="F121" t="n">
-        <v>1.32658064091</v>
+        <v>1.34781485183</v>
       </c>
       <c r="G121" t="n">
         <v>1.34893903671</v>
       </c>
       <c r="H121" t="n">
-        <v>0.0223583958032</v>
+        <v>0.00112418488353</v>
       </c>
     </row>
     <row r="122" spans="1:10">
@@ -3074,13 +3074,13 @@
         <v>61</v>
       </c>
       <c r="F122" t="n">
-        <v>1.15180109192</v>
+        <v>1.12542156452</v>
       </c>
       <c r="G122" t="n">
         <v>1.1306837319</v>
       </c>
       <c r="H122" t="n">
-        <v>-0.0211173600233</v>
+        <v>0.00526216737696</v>
       </c>
     </row>
     <row r="123" spans="1:10">
@@ -3088,13 +3088,13 @@
         <v>137</v>
       </c>
       <c r="F123" t="n">
-        <v>1.32658064091</v>
+        <v>1.34781485183</v>
       </c>
       <c r="G123" t="n">
         <v>1.34893903671</v>
       </c>
       <c r="H123" t="n">
-        <v>0.0223583958032</v>
+        <v>0.00112418488353</v>
       </c>
     </row>
     <row r="124" spans="1:10">
@@ -3102,13 +3102,13 @@
         <v>138</v>
       </c>
       <c r="F124" t="n">
-        <v>1.0909343795</v>
+        <v>1.11029862242</v>
       </c>
       <c r="G124" t="n">
         <v>1.12563152577</v>
       </c>
       <c r="H124" t="n">
-        <v>0.0346971462667</v>
+        <v>0.0153329033469</v>
       </c>
     </row>
     <row r="125" spans="1:10">
@@ -3116,13 +3116,13 @@
         <v>63</v>
       </c>
       <c r="F125" t="n">
-        <v>1.31037353417</v>
+        <v>1.33211027851</v>
       </c>
       <c r="G125" t="n">
         <v>1.32974065342</v>
       </c>
       <c r="H125" t="n">
-        <v>0.0193671192491</v>
+        <v>-0.00236962509052</v>
       </c>
     </row>
     <row r="126" spans="1:10">
@@ -3130,13 +3130,13 @@
         <v>64</v>
       </c>
       <c r="F126" t="n">
-        <v>0.51998632237</v>
+        <v>0.508245648867</v>
       </c>
       <c r="G126" t="n">
         <v>0.508251936679</v>
       </c>
       <c r="H126" t="n">
-        <v>-0.0117343856908</v>
+        <v>6.2878123297e-06</v>
       </c>
     </row>
     <row r="127" spans="1:10">
@@ -3144,13 +3144,13 @@
         <v>139</v>
       </c>
       <c r="F127" t="n">
-        <v>0.740153399232</v>
+        <v>0.7539584878659999</v>
       </c>
       <c r="G127" t="n">
         <v>0.757830919502</v>
       </c>
       <c r="H127" t="n">
-        <v>0.0176775202698</v>
+        <v>0.00387243163598</v>
       </c>
     </row>
     <row r="128" spans="1:10">
@@ -3158,13 +3158,13 @@
         <v>66</v>
       </c>
       <c r="F128" t="n">
-        <v>1.3157090422</v>
+        <v>1.29136388046</v>
       </c>
       <c r="G128" t="n">
         <v>1.28427079825</v>
       </c>
       <c r="H128" t="n">
-        <v>-0.031438243951</v>
+        <v>-0.00709308221064</v>
       </c>
     </row>
     <row r="129" spans="1:10">
@@ -3172,13 +3172,13 @@
         <v>140</v>
       </c>
       <c r="F129" t="n">
-        <v>1.1119078401</v>
+        <v>1.09169830677</v>
       </c>
       <c r="G129" t="n">
         <v>1.0882452004</v>
       </c>
       <c r="H129" t="n">
-        <v>-0.0236626396954</v>
+        <v>-0.00345310636515</v>
       </c>
     </row>
     <row r="130" spans="1:10">
@@ -3186,13 +3186,13 @@
         <v>141</v>
       </c>
       <c r="F130" t="n">
-        <v>1.28976963075</v>
+        <v>1.31079628805</v>
       </c>
       <c r="G130" t="n">
         <v>1.29841697541</v>
       </c>
       <c r="H130" t="n">
-        <v>0.008647344663060001</v>
+        <v>-0.0123793126366</v>
       </c>
     </row>
     <row r="131" spans="1:10">
@@ -3200,13 +3200,13 @@
         <v>68</v>
       </c>
       <c r="F131" t="n">
-        <v>1.1119078401</v>
+        <v>1.09169830677</v>
       </c>
       <c r="G131" t="n">
         <v>1.0882452004</v>
       </c>
       <c r="H131" t="n">
-        <v>-0.0236626396954</v>
+        <v>-0.00345310636515</v>
       </c>
     </row>
     <row r="132" spans="1:10">
@@ -3214,13 +3214,13 @@
         <v>142</v>
       </c>
       <c r="F132" t="n">
-        <v>1.3157090422</v>
+        <v>1.29136388046</v>
       </c>
       <c r="G132" t="n">
         <v>1.28427079825</v>
       </c>
       <c r="H132" t="n">
-        <v>-0.031438243951</v>
+        <v>-0.00709308221064</v>
       </c>
     </row>
     <row r="133" spans="1:10">
@@ -3228,13 +3228,13 @@
         <v>143</v>
       </c>
       <c r="F133" t="n">
-        <v>0.740153399232</v>
+        <v>0.7539584878659999</v>
       </c>
       <c r="G133" t="n">
         <v>0.757830919502</v>
       </c>
       <c r="H133" t="n">
-        <v>0.0176775202698</v>
+        <v>0.00387243163598</v>
       </c>
     </row>
     <row r="134" spans="1:10">
@@ -3242,13 +3242,13 @@
         <v>144</v>
       </c>
       <c r="F134" t="n">
-        <v>0.536432909213</v>
+        <v>0.545710923476</v>
       </c>
       <c r="G134" t="n">
         <v>0.533512967329</v>
       </c>
       <c r="H134" t="n">
-        <v>-0.00291994188374</v>
+        <v>-0.0121979561466</v>
       </c>
     </row>
     <row r="135" spans="1:10">
@@ -3256,13 +3256,13 @@
         <v>70</v>
       </c>
       <c r="F135" t="n">
-        <v>0.6747973981249999</v>
+        <v>0.687179174242</v>
       </c>
       <c r="G135" t="n">
         <v>0.675985180196</v>
       </c>
       <c r="H135" t="n">
-        <v>0.0011877820706</v>
+        <v>-0.0111939940462</v>
       </c>
     </row>
     <row r="136" spans="1:10">
@@ -3270,13 +3270,13 @@
         <v>145</v>
       </c>
       <c r="F136" t="n">
-        <v>0.967927045037</v>
+        <v>0.984686311592</v>
       </c>
       <c r="G136" t="n">
-        <v>0.986190636578</v>
+        <v>0.986190636579</v>
       </c>
       <c r="H136" t="n">
-        <v>0.0182635915413</v>
+        <v>0.00150432498658</v>
       </c>
     </row>
     <row r="137" spans="1:10">
@@ -3284,13 +3284,13 @@
         <v>146</v>
       </c>
       <c r="F137" t="n">
-        <v>1.2135475467</v>
+        <v>1.23228780065</v>
       </c>
       <c r="G137" t="n">
         <v>1.23071741327</v>
       </c>
       <c r="H137" t="n">
-        <v>0.0171698665709</v>
+        <v>-0.00157038737878</v>
       </c>
     </row>
     <row r="138" spans="1:10">
@@ -3298,13 +3298,13 @@
         <v>72</v>
       </c>
       <c r="F138" t="n">
-        <v>0.9847901815</v>
+        <v>1.00188841038</v>
       </c>
       <c r="G138" t="n">
-        <v>0.997305490064</v>
+        <v>0.997305490065</v>
       </c>
       <c r="H138" t="n">
-        <v>0.0125153085644</v>
+        <v>-0.00458292031539</v>
       </c>
     </row>
     <row r="139" spans="1:10">
@@ -3312,13 +3312,13 @@
         <v>147</v>
       </c>
       <c r="F139" t="n">
-        <v>1.2135475467</v>
+        <v>1.23228780065</v>
       </c>
       <c r="G139" t="n">
         <v>1.23071741327</v>
       </c>
       <c r="H139" t="n">
-        <v>0.0171698665709</v>
+        <v>-0.00157038737878</v>
       </c>
     </row>
     <row r="140" spans="1:10">
@@ -3326,13 +3326,13 @@
         <v>148</v>
       </c>
       <c r="F140" t="n">
-        <v>0.967927045037</v>
+        <v>0.984686311592</v>
       </c>
       <c r="G140" t="n">
-        <v>0.986190636578</v>
+        <v>0.986190636579</v>
       </c>
       <c r="H140" t="n">
-        <v>0.0182635915413</v>
+        <v>0.00150432498658</v>
       </c>
     </row>
     <row r="141" spans="1:10">
@@ -3340,13 +3340,13 @@
         <v>149</v>
       </c>
       <c r="F141" t="n">
-        <v>0.6747973981249999</v>
+        <v>0.687179174242</v>
       </c>
       <c r="G141" t="n">
         <v>0.675985180196</v>
       </c>
       <c r="H141" t="n">
-        <v>0.0011877820706</v>
+        <v>-0.0111939940462</v>
       </c>
     </row>
     <row r="142" spans="1:10">
@@ -3354,13 +3354,13 @@
         <v>150</v>
       </c>
       <c r="F142" t="n">
-        <v>0.536432909213</v>
+        <v>0.545710923476</v>
       </c>
       <c r="G142" t="n">
         <v>0.533512967329</v>
       </c>
       <c r="H142" t="n">
-        <v>-0.00291994188374</v>
+        <v>-0.0121979561466</v>
       </c>
     </row>
     <row r="143" spans="1:10">
@@ -3368,13 +3368,13 @@
         <v>74</v>
       </c>
       <c r="F143" t="n">
-        <v>0.536432909213</v>
+        <v>0.545710923476</v>
       </c>
       <c r="G143" t="n">
         <v>0.533512967329</v>
       </c>
       <c r="H143" t="n">
-        <v>-0.00291994188374</v>
+        <v>-0.0121979561466</v>
       </c>
     </row>
     <row r="144" spans="1:10">
@@ -3382,13 +3382,13 @@
         <v>151</v>
       </c>
       <c r="F144" t="n">
-        <v>0.740153399232</v>
+        <v>0.7539584878659999</v>
       </c>
       <c r="G144" t="n">
         <v>0.757830919502</v>
       </c>
       <c r="H144" t="n">
-        <v>0.0176775202698</v>
+        <v>0.00387243163598</v>
       </c>
     </row>
     <row r="145" spans="1:10">
@@ -3396,13 +3396,13 @@
         <v>152</v>
       </c>
       <c r="F145" t="n">
-        <v>1.14402073566</v>
+        <v>1.16332001126</v>
       </c>
       <c r="G145" t="n">
         <v>1.14482990906</v>
       </c>
       <c r="H145" t="n">
-        <v>0.000809173400702</v>
+        <v>-0.018490102199</v>
       </c>
     </row>
     <row r="146" spans="1:10">
@@ -3410,13 +3410,13 @@
         <v>75</v>
       </c>
       <c r="F146" t="n">
-        <v>0.8081335310809999</v>
+        <v>0.822605739677</v>
       </c>
       <c r="G146" t="n">
         <v>0.834624452678</v>
       </c>
       <c r="H146" t="n">
-        <v>0.026490921597</v>
+        <v>0.0120187130012</v>
       </c>
     </row>
     <row r="147" spans="1:10">
@@ -3424,13 +3424,13 @@
         <v>153</v>
       </c>
       <c r="F147" t="n">
-        <v>1.29924708381</v>
+        <v>1.21126960749</v>
       </c>
       <c r="G147" t="n">
         <v>1.18625799933</v>
       </c>
       <c r="H147" t="n">
-        <v>-0.112989084483</v>
+        <v>-0.0250116081629</v>
       </c>
     </row>
     <row r="148" spans="1:10">
@@ -3438,13 +3438,13 @@
         <v>154</v>
       </c>
       <c r="F148" t="n">
-        <v>0.8081335310809999</v>
+        <v>0.822605739677</v>
       </c>
       <c r="G148" t="n">
         <v>0.834624452678</v>
       </c>
       <c r="H148" t="n">
-        <v>0.026490921597</v>
+        <v>0.0120187130012</v>
       </c>
     </row>
     <row r="149" spans="1:10">
@@ -3452,13 +3452,13 @@
         <v>77</v>
       </c>
       <c r="F149" t="n">
-        <v>1.14402073566</v>
+        <v>1.16332001126</v>
       </c>
       <c r="G149" t="n">
         <v>1.14482990906</v>
       </c>
       <c r="H149" t="n">
-        <v>0.000809173400702</v>
+        <v>-0.018490102199</v>
       </c>
     </row>
     <row r="150" spans="1:10">
@@ -3466,13 +3466,13 @@
         <v>155</v>
       </c>
       <c r="F150" t="n">
-        <v>0.740153399232</v>
+        <v>0.7539584878659999</v>
       </c>
       <c r="G150" t="n">
         <v>0.757830919502</v>
       </c>
       <c r="H150" t="n">
-        <v>0.0176775202698</v>
+        <v>0.00387243163598</v>
       </c>
     </row>
     <row r="151" spans="1:10">
@@ -3480,13 +3480,13 @@
         <v>156</v>
       </c>
       <c r="F151" t="n">
-        <v>0.536432909213</v>
+        <v>0.545710923476</v>
       </c>
       <c r="G151" t="n">
         <v>0.533512967329</v>
       </c>
       <c r="H151" t="n">
-        <v>-0.00291994188374</v>
+        <v>-0.0121979561466</v>
       </c>
     </row>
     <row r="152" spans="1:10">
@@ -3494,13 +3494,13 @@
         <v>78</v>
       </c>
       <c r="F152" t="n">
-        <v>0.51998632237</v>
+        <v>0.508245648867</v>
       </c>
       <c r="G152" t="n">
         <v>0.508251936679</v>
       </c>
       <c r="H152" t="n">
-        <v>-0.0117343856908</v>
+        <v>6.2878123297e-06</v>
       </c>
     </row>
     <row r="153" spans="1:10">
@@ -3508,13 +3508,13 @@
         <v>157</v>
       </c>
       <c r="F153" t="n">
-        <v>0.622596162957</v>
+        <v>0.633570024496</v>
       </c>
       <c r="G153" t="n">
-        <v>0.635567531155</v>
+        <v>0.635567531156</v>
       </c>
       <c r="H153" t="n">
-        <v>0.0129713681985</v>
+        <v>0.00199750665966</v>
       </c>
     </row>
     <row r="154" spans="1:10">
@@ -3522,13 +3522,13 @@
         <v>158</v>
       </c>
       <c r="F154" t="n">
-        <v>0.690532719584</v>
+        <v>0.701599288685</v>
       </c>
       <c r="G154" t="n">
         <v>0.71034018188</v>
       </c>
       <c r="H154" t="n">
-        <v>0.0198074622957</v>
+        <v>0.008740893194859999</v>
       </c>
     </row>
     <row r="155" spans="1:10">
@@ -3536,13 +3536,13 @@
         <v>159</v>
       </c>
       <c r="F155" t="n">
-        <v>0.666216950391</v>
+        <v>0.678846256784</v>
       </c>
       <c r="G155" t="n">
         <v>0.691141798586</v>
       </c>
       <c r="H155" t="n">
-        <v>0.0249248481946</v>
+        <v>0.0122955418018</v>
       </c>
     </row>
     <row r="156" spans="1:10">
@@ -3550,13 +3550,13 @@
         <v>160</v>
       </c>
       <c r="F156" t="n">
-        <v>0.690532719584</v>
+        <v>0.701599288685</v>
       </c>
       <c r="G156" t="n">
         <v>0.71034018188</v>
       </c>
       <c r="H156" t="n">
-        <v>0.0198074622957</v>
+        <v>0.008740893194859999</v>
       </c>
     </row>
     <row r="157" spans="1:10">
@@ -3564,13 +3564,13 @@
         <v>161</v>
       </c>
       <c r="F157" t="n">
-        <v>0.622596162957</v>
+        <v>0.633570024496</v>
       </c>
       <c r="G157" t="n">
-        <v>0.635567531155</v>
+        <v>0.635567531156</v>
       </c>
       <c r="H157" t="n">
-        <v>0.0129713681985</v>
+        <v>0.00199750665966</v>
       </c>
     </row>
     <row r="158" spans="1:10">
@@ -3578,13 +3578,13 @@
         <v>162</v>
       </c>
       <c r="F158" t="n">
-        <v>0.51998632237</v>
+        <v>0.508245648867</v>
       </c>
       <c r="G158" t="n">
         <v>0.508251936679</v>
       </c>
       <c r="H158" t="n">
-        <v>-0.0117343856908</v>
+        <v>6.2878123297e-06</v>
       </c>
     </row>
   </sheetData>

</xml_diff>